<commit_message>
Basics and Species part added to the Editor
</commit_message>
<xml_diff>
--- a/doc/options.xlsx
+++ b/doc/options.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vizha\Documents\javascript\star-trek-adventures\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E89AD8-2275-4FD3-904A-BC0D4B31AAF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D12E82-591C-4A6C-88EA-96BCC36A9410}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{D445157F-2575-4AC8-8D6C-5820EF4A9821}"/>
   </bookViews>
@@ -1755,10 +1755,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FCF0B8B-6D73-4E71-92BE-AB1F2BD62168}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1769,7 +1769,7 @@
     <col min="5" max="5" width="38.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1782,8 +1782,11 @@
       <c r="D1" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1796,8 +1799,11 @@
       <c r="D2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1810,8 +1816,11 @@
       <c r="D3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1824,8 +1833,11 @@
       <c r="D4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1838,8 +1850,11 @@
       <c r="D5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1852,8 +1867,11 @@
       <c r="D6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1866,39 +1884,7 @@
       <c r="D7" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="E7" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Environment added to the editor Major structural refactoring
</commit_message>
<xml_diff>
--- a/doc/options.xlsx
+++ b/doc/options.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vizha\Documents\javascript\star-trek-adventures\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D12E82-591C-4A6C-88EA-96BCC36A9410}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8109B670-3156-48B3-8356-6E275EF17EF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{D445157F-2575-4AC8-8D6C-5820EF4A9821}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="255">
   <si>
     <t>Andorian</t>
   </si>
@@ -774,6 +774,39 @@
   </si>
   <si>
     <t>choose 1 Discipline</t>
+  </si>
+  <si>
+    <t>1,4</t>
+  </si>
+  <si>
+    <t>3,5</t>
+  </si>
+  <si>
+    <t>0,2</t>
+  </si>
+  <si>
+    <t>0,3</t>
+  </si>
+  <si>
+    <t>0,3,4</t>
+  </si>
+  <si>
+    <t>2,4,5</t>
+  </si>
+  <si>
+    <t>1,3,5</t>
+  </si>
+  <si>
+    <t>0,1,2</t>
+  </si>
+  <si>
+    <t>0,1,2,3,4,5</t>
+  </si>
+  <si>
+    <t>"Environment":[</t>
+  </si>
+  <si>
+    <t>]</t>
   </si>
 </sst>
 </file>
@@ -1132,7 +1165,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1755,10 +1788,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FCF0B8B-6D73-4E71-92BE-AB1F2BD62168}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1769,7 +1802,7 @@
     <col min="5" max="5" width="38.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1786,7 +1819,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1803,7 +1836,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1820,7 +1853,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1837,7 +1870,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1854,7 +1887,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1871,7 +1904,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1886,6 +1919,151 @@
       </c>
       <c r="E7" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>242</v>
+      </c>
+      <c r="D9" t="s">
+        <v>243</v>
+      </c>
+      <c r="E9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>248</v>
+      </c>
+      <c r="E10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" ref="F10" si="0">_xlfn.CONCAT("{""name"":""",B10,""",roll:",A10, ",""attributes"":[",C10,"],""disciplines"":[",D10,"],""exValue"":""",E10,"""},")</f>
+        <v>{"name":"Homeworld",roll:1,"attributes":[],"disciplines":[0,3,4],"exValue":"Body and Mind Alike Must Be Healthy"},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>244</v>
+      </c>
+      <c r="D11" t="s">
+        <v>248</v>
+      </c>
+      <c r="E11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" t="str">
+        <f>_xlfn.CONCAT("{""name"":""",B11,""",roll:",A11, ",""attributes"":[",C11,"],""disciplines"":[",D11,"],""exValue"":""",E11,"""},")</f>
+        <v>{"name":"Busy Colony",roll:2,"attributes":[1,4],"disciplines":[0,3,4],"exValue":"Most Comfortable in a Crowd"},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>245</v>
+      </c>
+      <c r="D12" t="s">
+        <v>249</v>
+      </c>
+      <c r="E12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" ref="F12:F15" si="1">_xlfn.CONCAT("{""name"":""",B12,""",roll:",A12, ",""attributes"":[",C12,"],""disciplines"":[",D12,"],""exValue"":""",E12,"""},")</f>
+        <v>{"name":"Isolated Colony",roll:3,"attributes":[3,5],"disciplines":[2,4,5],"exValue":"Engineer at Heart"},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>246</v>
+      </c>
+      <c r="D13" t="s">
+        <v>250</v>
+      </c>
+      <c r="E13" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="1"/>
+        <v>{"name":"Frontier Colony",roll:4,"attributes":[0,2],"disciplines":[1,3,5],"exValue":"No Stranger to Violence"},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>247</v>
+      </c>
+      <c r="D14" t="s">
+        <v>251</v>
+      </c>
+      <c r="E14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="1"/>
+        <v>{"name":"Starship or Starbase",roll:5,"attributes":[0,3],"disciplines":[0,1,2],"exValue":"A Starship is a Home, it’s Crew a Family"},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>252</v>
+      </c>
+      <c r="E15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="1"/>
+        <v>{"name":"Another Species' World",roll:6,"attributes":[],"disciplines":[0,1,2,3,4,5],"exValue":"Emotion in a Crisis only Makes Things Worse"},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F16" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>